<commit_message>
Initial checklist template defined and tested; still need to add more rule options.
</commit_message>
<xml_diff>
--- a/src/checklist/test/TestGridMatch.xlsx
+++ b/src/checklist/test/TestGridMatch.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="360" windowWidth="23720" windowHeight="21680" tabRatio="500"/>
+    <workbookView xWindow="20620" yWindow="3440" windowWidth="17480" windowHeight="21680" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="TestGridMatch.csv" sheetId="1" r:id="rId1"/>
@@ -35,171 +35,227 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="109">
-  <si>
-    <t>wfdesc</t>
-  </si>
-  <si>
-    <t>wf4ever</t>
-  </si>
-  <si>
-    <t>minim</t>
-  </si>
-  <si>
-    <t>http://www.w3.org/1999/02/22-rdf-syntax-ns#</t>
-  </si>
-  <si>
-    <t>http://www.w3.org/2000/01/rdf-schema#</t>
-  </si>
-  <si>
-    <t>http://www.w3.org/2002/07/owl#</t>
-  </si>
-  <si>
-    <t>http://www.w3.org/2001/XMLSchema#</t>
-  </si>
-  <si>
-    <t>http://www.w3.org/XML/1998/namespace</t>
-  </si>
-  <si>
-    <t>http://www.w3.org/2004/03/trix/rdfg-1/</t>
-  </si>
-  <si>
-    <t>http://www.openarchives.org/ore/terms/</t>
-  </si>
-  <si>
-    <t>#experiment_complete_model</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>#wf_accessible_model</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>#experiment_complete_model</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>#RO_has_hypothesys</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>#RO_has_sketch</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>#WF_accessible</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>#WF_accessible</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>#WF_services_accessible</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>#RO_has_inputdata</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>#RO_has_conclusion</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>#RO_has_hypothesys</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>#WF_accessible</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>#WF_services_accessible</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>One or more web services used by a workflow are inaccessible, including &lt;a href="%(pruri)s"&gt;&lt;i&gt;%(prlab)s&lt;/i&gt;&lt;/a&gt;</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>No web services are referenced by any workflow</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>050</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>060</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Exists:</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>RO should contain a resource describing the hypothesis the experiment is intended to test</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Workflow design sketch is present</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Workflow design sketch is not present</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>?sketch rdf:type roterms:Sketch</t>
-  </si>
-  <si>
-    <t>ForEach:</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="110">
+  <si>
+    <t>The RO must specify input data that is used by the workflow</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">The RO should contain a resource that describes outcomes and conclusions obtained by running the workflow. </t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rule:</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Experiment hypothesis is not present</t>
+  </si>
+  <si>
+    <t>Pass:</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>?hypothesis rdf:type roterms:Hypothesis</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Experiment hypothesis is present</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>?wf rdf:type wfdesc:Workflow ;
   rdfs:label ?wflab ;
   wfdesc:hasWorkflowDefinition ?wfdef</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>#RO_has_hypothesis</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>#RO_has_hypothesis</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Model to test workflow accessible item in isolation</t>
+  </si>
+  <si>
+    <t>xsd</t>
+  </si>
+  <si>
+    <t>xml</t>
+  </si>
+  <si>
+    <t>?wfbundle roterms:inputSelected ?inputdata</t>
+  </si>
+  <si>
+    <t>Input data is present</t>
+  </si>
+  <si>
+    <t>Input data is not present</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>?conclusion rdf:type roterms:Conclusions</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Experiment conclusions are present</t>
+  </si>
+  <si>
+    <t>Experiment conclusions are not present</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>All workflow definitions are accessible</t>
+  </si>
+  <si>
+    <t>wfdesc</t>
+  </si>
+  <si>
+    <t>wf4ever</t>
+  </si>
+  <si>
+    <t>minim</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/1999/02/22-rdf-syntax-ns#</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/2000/01/rdf-schema#</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/2002/07/owl#</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/2001/XMLSchema#</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/XML/1998/namespace</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/2004/03/trix/rdfg-1/</t>
+  </si>
+  <si>
+    <t>http://www.openarchives.org/ore/terms/</t>
+  </si>
+  <si>
+    <t>#experiment_complete_model</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>#wf_accessible_model</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>#experiment_complete_model</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>#RO_has_sketch</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>#WF_accessible</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>#WF_accessible</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>#WF_services_accessible</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>#RO_has_inputdata</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>#RO_has_conclusion</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>#WF_accessible</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>#WF_services_accessible</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>One or more web services used by a workflow are inaccessible, including &lt;a href="%(pruri)s"&gt;&lt;i&gt;%(prlab)s&lt;/i&gt;&lt;/a&gt;</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>No web services are referenced by any workflow</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>050</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>060</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Exists:</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>RO should contain a resource describing the hypothesis the experiment is intended to test</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Workflow design sketch is present</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Workflow design sketch is not present</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>?sketch rdf:type roterms:Sketch</t>
+  </si>
+  <si>
+    <t>ForEach:</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>{+wfdef}</t>
   </si>
   <si>
     <t>IsLive:</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Prefixes:</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>{+targetro}</t>
   </si>
   <si>
     <t>Target</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Purpose</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Description</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Checklist:</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>ready-to-release</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Model</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>rdfs</t>
@@ -209,218 +265,18 @@
   </si>
   <si>
     <t>rdf</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>The RO must specify input data that is used by the workflow</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">The RO should contain a resource that describes outcomes and conclusions obtained by running the workflow. </t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Rule:</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>?hypothesis rdf:type roterms:Hypothesis</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Experiment hypothesis is present</t>
-  </si>
-  <si>
-    <t>Experiment hypothesis is not present</t>
-  </si>
-  <si>
-    <t>Pass:</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Fail:</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>@@NOTE: there is a shortcoming in the present Minim model and implementation that means there is no way to add new prefixes to those predefined in the minim evaluation code.  Noted as technical debt fix.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Define rules to test individual requirements</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>010</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>020</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>030</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>040</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Model:</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Items:</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>This model defines information that must be satisfied by the target RO for the target RO to be considered a complete and fully-described workflow experiment.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Level</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SHOULD</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Rule</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>MUST</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>MUST</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>MUST</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>rdfg</t>
-  </si>
-  <si>
-    <t>ore</t>
-  </si>
-  <si>
-    <t>ao</t>
-  </si>
-  <si>
-    <t>dcterms</t>
-  </si>
-  <si>
-    <t>foaf</t>
-  </si>
-  <si>
-    <t>ro</t>
-  </si>
-  <si>
-    <t>wfprov</t>
-  </si>
-  <si>
-    <t>RO should contain a resource that is a high level sketch of the workflow that is used to test the hypothesys</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>The RO must contain an accessible workflow definition</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>All services used by the workflow must be live</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://purl.org/ao/</t>
-  </si>
-  <si>
-    <t>http://purl.org/dc/terms/</t>
-  </si>
-  <si>
-    <t>http://xmlns.com/foaf/0.1/</t>
-  </si>
-  <si>
-    <t>http://purl.org/wf4ever/ro#</t>
-  </si>
-  <si>
-    <t>http://purl.org/wf4ever/wfprov#</t>
-  </si>
-  <si>
-    <t>http://purl.org/wf4ever/wfdesc#</t>
-  </si>
-  <si>
-    <t>http://purl.org/wf4ever/wf4ever#</t>
-  </si>
-  <si>
-    <t>http://purl.org/minim/minim#</t>
-  </si>
-  <si>
-    <t>Prefix</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>URI</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>wf-accessible</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Checklist to test workflow accessible item in isolation</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Checklist to be satisfied if the target RO is to be considered a complete and fully-described workflow experiment.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Model to test workflow accessible item in isolation</t>
-  </si>
-  <si>
-    <t>xsd</t>
-  </si>
-  <si>
-    <t>xml</t>
-  </si>
-  <si>
-    <t>?wfbundle roterms:inputSelected ?inputdata</t>
-  </si>
-  <si>
-    <t>Input data is present</t>
-  </si>
-  <si>
-    <t>Input data is not present</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>?conclusion rdf:type roterms:Conclusions</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Experiment conclusions are present</t>
-  </si>
-  <si>
-    <t>Experiment conclusions are not present</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>All workflow definitions are accessible</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>The definition for workflow &lt;i&gt;%(wflab)s&lt;/i&gt; is not accessible</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>No workflow definitions are present</t>
   </si>
   <si>
     <t>None:</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>?pr rdf:type wfdesc:Process ;
@@ -428,23 +284,177 @@
     { ?pr wf4ever:serviceURI ?pruri }
   UNION
     { ?pr wf4ever:wsdlURI ?pruri }</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>{+pruri}</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>All web services used by workflows are accessible</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>End:</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Checklists:</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fail:</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>@@NOTE: there is a shortcoming in the present Minim model and implementation that means there is no way to add new prefixes to those predefined in the minim evaluation code.  Noted as technical debt fix.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Define rules to test individual requirements</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>010</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>020</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>030</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>040</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Model:</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Items:</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>This model defines information that must be satisfied by the target RO for the target RO to be considered a complete and fully-described workflow experiment.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Level</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>SHOULD</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rule</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>MUST</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>MUST</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>MUST</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>rdfg</t>
+  </si>
+  <si>
+    <t>ore</t>
+  </si>
+  <si>
+    <t>ao</t>
+  </si>
+  <si>
+    <t>dcterms</t>
+  </si>
+  <si>
+    <t>foaf</t>
+  </si>
+  <si>
+    <t>ro</t>
+  </si>
+  <si>
+    <t>wfprov</t>
+  </si>
+  <si>
+    <t>RO should contain a resource that is a high level sketch of the workflow that is used to test the hypothesys</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>The RO must contain an accessible workflow definition</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>All services used by the workflow must be live</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://purl.org/ao/</t>
+  </si>
+  <si>
+    <t>http://purl.org/dc/terms/</t>
+  </si>
+  <si>
+    <t>http://xmlns.com/foaf/0.1/</t>
+  </si>
+  <si>
+    <t>http://purl.org/wf4ever/ro#</t>
+  </si>
+  <si>
+    <t>http://purl.org/wf4ever/wfprov#</t>
+  </si>
+  <si>
+    <t>http://purl.org/wf4ever/wfdesc#</t>
+  </si>
+  <si>
+    <t>http://purl.org/wf4ever/wf4ever#</t>
+  </si>
+  <si>
+    <t>http://purl.org/minim/minim#</t>
+  </si>
+  <si>
+    <t>Prefix</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>URI</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>wf-accessible</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Checklist to test workflow accessible item in isolation</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Checklist to be satisfied if the target RO is to be considered a complete and fully-described workflow experiment.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
       <name val="Verdana"/>
     </font>
@@ -482,25 +492,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -512,6 +522,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -848,15 +859,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:G69"/>
+  <dimension ref="A1:G71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66"/>
+    <sheetView showFormulas="1" tabSelected="1" topLeftCell="A20" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" customWidth="1"/>
     <col min="2" max="2" width="10.140625" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" customWidth="1"/>
@@ -867,185 +878,185 @@
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" ht="39">
       <c r="A1" s="4" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>89</v>
+        <v>106</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
       <c r="F1" s="10" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:7">
       <c r="B2" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="B3" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="B4" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="B5" t="s">
-        <v>94</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="B6" t="s">
-        <v>95</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="B7" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="B8" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="B9" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="C9" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="B10" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="C10" t="s">
-        <v>81</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="B11" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="C11" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="B12" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="C12" t="s">
-        <v>83</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="B13" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="C13" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="B14" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>85</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="B15" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>86</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="B16" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="C16" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="1" customFormat="1">
       <c r="A18" s="1" t="s">
-        <v>41</v>
+        <v>70</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:7" s="2" customFormat="1" ht="26">
       <c r="B19" s="2" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
       <c r="G19" s="3"/>
     </row>
     <row r="20" spans="1:7" s="2" customFormat="1">
       <c r="B20" s="2" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>90</v>
+        <v>107</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>91</v>
+        <v>108</v>
       </c>
       <c r="G20" s="9"/>
     </row>
@@ -1055,400 +1066,404 @@
     </row>
     <row r="22" spans="1:7" s="4" customFormat="1" ht="39">
       <c r="A22" s="4" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="6" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="G22" s="5"/>
     </row>
     <row r="23" spans="1:7" s="1" customFormat="1">
       <c r="A23" s="1" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:7" s="2" customFormat="1" ht="26">
       <c r="A24" s="7" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:7" s="2" customFormat="1" ht="26">
       <c r="A25" s="7" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:7" s="2" customFormat="1">
       <c r="A26" s="7" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>78</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:7" s="2" customFormat="1">
       <c r="A27" s="7" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:7" s="2" customFormat="1">
       <c r="A28" s="7" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>47</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:7" s="2" customFormat="1" ht="26">
       <c r="A29" s="7" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>48</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:7" s="4" customFormat="1">
       <c r="A31" s="4" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
       <c r="F31" s="6" t="s">
-        <v>93</v>
+        <v>10</v>
       </c>
       <c r="G31" s="5"/>
     </row>
     <row r="32" spans="1:7" s="1" customFormat="1">
       <c r="A32" s="1" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
     </row>
     <row r="33" spans="1:6" s="2" customFormat="1">
       <c r="A33" s="7" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>78</v>
+        <v>95</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="1" customFormat="1">
       <c r="A35" s="1" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="2" customFormat="1">
       <c r="A37" s="4" t="s">
-        <v>49</v>
+        <v>2</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="F37" s="3"/>
     </row>
     <row r="38" spans="1:6">
       <c r="B38" s="1" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="C38" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="B39" s="1" t="s">
-        <v>53</v>
+        <v>4</v>
       </c>
       <c r="C39" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="B40" s="1" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="C40" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:6" s="2" customFormat="1">
       <c r="A42" s="4" t="s">
-        <v>49</v>
+        <v>2</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="F42" s="3"/>
     </row>
     <row r="43" spans="1:6">
       <c r="B43" s="1" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="C43" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="B44" s="1" t="s">
-        <v>53</v>
+        <v>4</v>
       </c>
       <c r="C44" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="B45" s="1" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="C45" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
     </row>
     <row r="47" spans="1:6" s="2" customFormat="1">
       <c r="A47" s="4" t="s">
-        <v>49</v>
+        <v>2</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="F47" s="3"/>
     </row>
     <row r="48" spans="1:6" s="2" customFormat="1" ht="40" customHeight="1">
       <c r="B48" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C48" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D48" s="11"/>
-      <c r="E48" s="11"/>
+        <v>50</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D48" s="12"/>
+      <c r="E48" s="12"/>
     </row>
     <row r="49" spans="1:6">
       <c r="B49" s="1" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="B50" s="1" t="s">
-        <v>53</v>
+        <v>4</v>
       </c>
       <c r="C50" t="s">
-        <v>102</v>
+        <v>19</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="B51" s="1" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="C51" t="s">
-        <v>103</v>
+        <v>63</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="B52" s="1" t="s">
-        <v>105</v>
+        <v>65</v>
       </c>
       <c r="C52" t="s">
-        <v>104</v>
+        <v>64</v>
       </c>
     </row>
     <row r="54" spans="1:6" s="2" customFormat="1">
       <c r="A54" s="4" t="s">
-        <v>49</v>
+        <v>2</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="F54" s="3"/>
     </row>
     <row r="55" spans="1:6" s="2" customFormat="1" ht="66" customHeight="1">
       <c r="B55" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C55" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="D55" s="11"/>
-      <c r="E55" s="11"/>
+        <v>50</v>
+      </c>
+      <c r="C55" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D55" s="12"/>
+      <c r="E55" s="12"/>
     </row>
     <row r="56" spans="1:6">
       <c r="B56" s="1" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>107</v>
+        <v>67</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="B57" s="1" t="s">
-        <v>53</v>
+        <v>4</v>
       </c>
       <c r="C57" t="s">
-        <v>108</v>
+        <v>68</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="B58" s="1" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="C58" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="B59" s="1" t="s">
-        <v>105</v>
+        <v>65</v>
       </c>
       <c r="C59" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
     </row>
     <row r="61" spans="1:6" s="2" customFormat="1">
       <c r="A61" s="4" t="s">
-        <v>49</v>
+        <v>2</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="F61" s="3"/>
     </row>
     <row r="62" spans="1:6">
       <c r="B62" s="1" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="C62" t="s">
-        <v>96</v>
+        <v>13</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="B63" s="1" t="s">
-        <v>53</v>
+        <v>4</v>
       </c>
       <c r="C63" t="s">
-        <v>97</v>
+        <v>14</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="B64" s="1" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="C64" t="s">
-        <v>98</v>
+        <v>15</v>
       </c>
     </row>
     <row r="66" spans="1:6" s="2" customFormat="1">
       <c r="A66" s="4" t="s">
-        <v>49</v>
+        <v>2</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="F66" s="3"/>
     </row>
     <row r="67" spans="1:6">
       <c r="B67" s="1" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="C67" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c r="B68" s="1" t="s">
-        <v>53</v>
+        <v>4</v>
       </c>
       <c r="C68" t="s">
-        <v>100</v>
+        <v>17</v>
       </c>
     </row>
     <row r="69" spans="1:6">
       <c r="B69" s="1" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="C69" t="s">
-        <v>101</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71" s="11" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="2">
     <mergeCell ref="C48:E48"/>
     <mergeCell ref="C55:E55"/>
   </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.39000000000000007" right="0.39000000000000007" top="0.39000000000000007" bottom="0.2" header="0.39000000000000007" footer="0.2"/>
   <rowBreaks count="1" manualBreakCount="1">
     <brk id="34" max="16383" man="1"/>

</xml_diff>